<commit_message>
Auxillary output from ELC_DMD process added with corresponding changes across documents (Scenario EXP file and SubRes DK price)'
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_DKprices.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_DKprices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_03\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_03\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCA3291-18A2-4612-833C-01F26E826667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56902A1A-099B-48D9-A1F7-878138B89D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>EXP</t>
   </si>
   <si>
-    <t>Export of electricity to Denmark West</t>
-  </si>
-  <si>
     <t>PJ</t>
   </si>
   <si>
@@ -157,7 +154,10 @@
     <t>*IMP</t>
   </si>
   <si>
-    <t>ELC_DEM</t>
+    <t>ELC_PRIS</t>
+  </si>
+  <si>
+    <t>Sale of electricity to Denmark West</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
   <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,41 +923,41 @@
         <v>21</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -977,7 +977,7 @@
   <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +988,7 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
@@ -996,36 +996,36 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9">
@@ -1043,10 +1043,10 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">

</xml_diff>

<commit_message>
Bringing remote up to date
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_DKprices.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_DKprices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_03\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475ECA81-B13F-4E8C-88DF-51EF5B4C3088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110ED1C3-5868-4F6F-9CDA-8999B9D87C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -880,8 +880,8 @@
   </sheetPr>
   <dimension ref="B1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,8 +979,8 @@
   </sheetPr>
   <dimension ref="B1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G3" s="9">
         <v>2022</v>

</xml_diff>